<commit_message>
Medición del tiempo de ejecución de algoritmos de ordenamiento
</commit_message>
<xml_diff>
--- a/talleres/taller2/Taller_2.xlsx
+++ b/talleres/taller2/Taller_2.xlsx
@@ -11,14 +11,13 @@
     <sheet name="Selección" sheetId="1" r:id="rId2"/>
     <sheet name="Inserción(peor)" sheetId="2" r:id="rId3"/>
     <sheet name="Inserción(mejor)" sheetId="3" r:id="rId4"/>
-    <sheet name="Hoja1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Ciencias I</t>
   </si>
@@ -67,9 +66,6 @@
   <si>
     <t>T(n)=(3n-3)/2</t>
   </si>
-  <si>
-    <t>SizeOf</t>
-  </si>
 </sst>
 </file>
 
@@ -78,9 +74,9 @@
   <numFmts count="5">
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -131,11 +127,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -146,22 +141,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -173,6 +154,14 @@
       <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -191,6 +180,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -199,9 +210,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -209,16 +219,17 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -230,25 +241,10 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -262,12 +258,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -297,7 +287,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -309,127 +335,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -447,13 +359,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -491,6 +487,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -502,21 +507,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -547,11 +537,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -568,122 +564,122 @@
   <cellStyleXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -692,20 +688,20 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -715,34 +711,33 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -848,7 +843,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="" altLang="en-US"/>
+              <a:rPr lang="en-US" altLang="en-US"/>
               <a:t>T</a:t>
             </a:r>
             <a:r>
@@ -1238,10 +1233,10 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="" altLang="en-US"/>
+              <a:rPr lang="en-US" altLang="en-US"/>
               <a:t>Chrono</a:t>
             </a:r>
-            <a:endParaRPr lang="" altLang="en-US"/>
+            <a:endParaRPr lang="en-US" altLang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1626,10 +1621,10 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="" altLang="en-US"/>
+              <a:rPr lang="en-US" altLang="en-US"/>
               <a:t>Chrono</a:t>
             </a:r>
-            <a:endParaRPr lang="" altLang="en-US"/>
+            <a:endParaRPr lang="en-US" altLang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -2024,14 +2019,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="" altLang="en-US"/>
+              <a:rPr lang="en-US" altLang="en-US"/>
               <a:t>T</a:t>
             </a:r>
             <a:r>
               <a:t>(</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="" altLang="en-US"/>
+              <a:rPr lang="en-US" altLang="en-US"/>
               <a:t>n</a:t>
             </a:r>
             <a:r>
@@ -2421,10 +2416,10 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="" altLang="en-US"/>
+              <a:rPr lang="en-US" altLang="en-US"/>
               <a:t>Chrono</a:t>
             </a:r>
-            <a:endParaRPr lang="" altLang="en-US"/>
+            <a:endParaRPr lang="en-US" altLang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -2810,7 +2805,7 @@
               <a:t>T(</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="" altLang="en-US"/>
+              <a:rPr lang="en-US" altLang="en-US"/>
               <a:t>n</a:t>
             </a:r>
             <a:r>
@@ -3121,768 +3116,6 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="547212975"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr lang="en-US"/>
-      </a:pPr>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="zh-CN"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>"f(n)"</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>f(n)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:delete val="1"/>
-          </c:dLbls>
-          <c:cat>
-            <c:numRef>
-              <c:f>Selección!$C$5:$C$24</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
-                <c:pt idx="0">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>95</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>100</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Selección!$E$5:$E$24</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
-                <c:pt idx="0">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>54</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>119</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>209</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>324</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>464</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>629</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>819</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1034</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1274</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1539</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1829</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2144</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2484</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2849</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>3239</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>3654</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>4094</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>4559</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>5049</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="0"/>
-        <c:smooth val="0"/>
-        <c:axId val="493395919"/>
-        <c:axId val="493397167"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="493395919"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="493397167"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="493397167"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="493395919"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr lang="en-US"/>
-      </a:pPr>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="zh-CN"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>"SizeOf"</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>SizeOf</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:delete val="1"/>
-          </c:dLbls>
-          <c:cat>
-            <c:numRef>
-              <c:f>Selección!$C$5:$C$24</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
-                <c:pt idx="0">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>95</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>100</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Selección!$D$5:$D$24</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
-                <c:pt idx="0">
-                  <c:v>0.000561</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.001343</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.001583</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.002394</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.003115</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.003907</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.00529</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.006502</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.008015</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.009588</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.011382</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.013385</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.015489</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.017673</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.020138</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.022693</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.025358</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.028333</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.031218</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.034535</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="0"/>
-        <c:smooth val="0"/>
-        <c:axId val="539451487"/>
-        <c:axId val="539454399"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="539451487"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="539454399"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="539454399"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="539451487"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4170,86 +3403,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -6831,1038 +5984,6 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8714,71 +6835,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame>
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="4410075" y="2738120"/>
-        <a:ext cx="6286500" cy="2314575"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame>
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Gráfico 2"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="4410075" y="394970"/>
-        <a:ext cx="6286500" cy="2343150"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
@@ -9130,7 +7186,7 @@
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
-      <c r="L8" s="14"/>
+      <c r="L8" s="13"/>
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
     </row>
@@ -9145,7 +7201,7 @@
       <c r="I9" s="10"/>
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
-      <c r="L9" s="12"/>
+      <c r="L9" s="1"/>
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
     </row>
@@ -9160,7 +7216,7 @@
       <c r="I10" s="11"/>
       <c r="J10" s="8"/>
       <c r="K10" s="9"/>
-      <c r="L10" s="12"/>
+      <c r="L10" s="1"/>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
     </row>
@@ -9175,7 +7231,7 @@
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
       <c r="K11" s="9"/>
-      <c r="L11" s="12"/>
+      <c r="L11" s="1"/>
       <c r="M11" s="5"/>
       <c r="N11" s="5"/>
     </row>
@@ -9188,18 +7244,18 @@
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
       <c r="K12" s="9"/>
-      <c r="L12" s="12"/>
+      <c r="L12" s="1"/>
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
     </row>
     <row r="13" spans="4:14">
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
@@ -9208,11 +7264,11 @@
     <row r="14" spans="4:14">
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
-      <c r="F14" s="12"/>
+      <c r="F14" s="1"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
-      <c r="J14" s="15"/>
+      <c r="J14" s="14"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
@@ -9224,8 +7280,8 @@
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
@@ -9262,7 +7318,7 @@
   <dimension ref="C3:E24"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" outlineLevelCol="4"/>
@@ -9271,11 +7327,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:5">
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" spans="3:5">
       <c r="C4" t="s">
@@ -9543,7 +7599,7 @@
   <sheetPr/>
   <dimension ref="C4:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B3" workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
@@ -9553,11 +7609,11 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:5">
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
     </row>
     <row r="5" spans="3:5">
       <c r="C5" t="s">
@@ -9825,8 +7881,8 @@
   <sheetPr/>
   <dimension ref="C2:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="D3" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" outlineLevelCol="7"/>
@@ -9835,19 +7891,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:8">
-      <c r="C2" s="2"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
     </row>
     <row r="4" spans="3:5">
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
     </row>
     <row r="5" spans="3:5">
       <c r="C5" t="s">
@@ -10110,283 +8166,4 @@
   <headerFooter/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="B2:D23"/>
-  <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" outlineLevelCol="3"/>
-  <sheetData>
-    <row r="2" spans="2:4">
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="2:4">
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4">
-      <c r="B4">
-        <v>5</v>
-      </c>
-      <c r="C4">
-        <v>0.000731</v>
-      </c>
-      <c r="D4">
-        <f>(B4^2+B4)/2-1</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4">
-      <c r="B5">
-        <v>10</v>
-      </c>
-      <c r="C5">
-        <v>0.001643</v>
-      </c>
-      <c r="D5">
-        <f t="shared" ref="D5:D23" si="0">(B5^2+B5)/2-1</f>
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4">
-      <c r="B6">
-        <v>15</v>
-      </c>
-      <c r="C6">
-        <v>0.002605</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
-        <v>119</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4">
-      <c r="B7">
-        <v>20</v>
-      </c>
-      <c r="C7">
-        <v>0.003286</v>
-      </c>
-      <c r="D7">
-        <f t="shared" si="0"/>
-        <v>209</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4">
-      <c r="B8">
-        <v>25</v>
-      </c>
-      <c r="C8">
-        <v>0.004118</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
-        <v>324</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4">
-      <c r="B9">
-        <v>30</v>
-      </c>
-      <c r="C9">
-        <v>0.00526</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>464</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4">
-      <c r="B10">
-        <v>35</v>
-      </c>
-      <c r="C10">
-        <v>0.006442</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="0"/>
-        <v>629</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4">
-      <c r="B11">
-        <v>40</v>
-      </c>
-      <c r="C11">
-        <v>0.008095</v>
-      </c>
-      <c r="D11">
-        <f t="shared" si="0"/>
-        <v>819</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4">
-      <c r="B12">
-        <v>45</v>
-      </c>
-      <c r="C12">
-        <v>0.009888</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="0"/>
-        <v>1034</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4">
-      <c r="B13">
-        <v>50</v>
-      </c>
-      <c r="C13">
-        <v>0.011982</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="0"/>
-        <v>1274</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4">
-      <c r="B14">
-        <v>55</v>
-      </c>
-      <c r="C14">
-        <v>0.014186</v>
-      </c>
-      <c r="D14">
-        <f t="shared" si="0"/>
-        <v>1539</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4">
-      <c r="B15">
-        <v>60</v>
-      </c>
-      <c r="C15">
-        <v>0.016541</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="0"/>
-        <v>1829</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4">
-      <c r="B16">
-        <v>65</v>
-      </c>
-      <c r="C16">
-        <v>0.019366</v>
-      </c>
-      <c r="D16">
-        <f t="shared" si="0"/>
-        <v>2144</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4">
-      <c r="B17">
-        <v>70</v>
-      </c>
-      <c r="C17">
-        <v>0.022001</v>
-      </c>
-      <c r="D17">
-        <f t="shared" si="0"/>
-        <v>2484</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4">
-      <c r="B18">
-        <v>75</v>
-      </c>
-      <c r="C18">
-        <v>0.025106</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="0"/>
-        <v>2849</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4">
-      <c r="B19">
-        <v>80</v>
-      </c>
-      <c r="C19">
-        <v>0.029304</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="0"/>
-        <v>3239</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4">
-      <c r="B20">
-        <v>85</v>
-      </c>
-      <c r="C20">
-        <v>0.032441</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="0"/>
-        <v>3654</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4">
-      <c r="B21">
-        <v>90</v>
-      </c>
-      <c r="C21">
-        <v>0.077574</v>
-      </c>
-      <c r="D21">
-        <f t="shared" si="0"/>
-        <v>4094</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4">
-      <c r="B22">
-        <v>95</v>
-      </c>
-      <c r="C22">
-        <v>0.041477</v>
-      </c>
-      <c r="D22">
-        <f t="shared" si="0"/>
-        <v>4559</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4">
-      <c r="B23">
-        <v>100</v>
-      </c>
-      <c r="C23">
-        <v>0.04842</v>
-      </c>
-      <c r="D23">
-        <f t="shared" si="0"/>
-        <v>5049</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B2:D2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>